<commit_message>
add Flask warning if used in backcast mode
- this would have helped with the output difference Fred and Andy had for request 866
</commit_message>
<xml_diff>
--- a/tests/request-issues.xlsx
+++ b/tests/request-issues.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andybega/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andybega/Work/SAGE-ward-share/basil-ts/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{881DAD76-766F-CA43-8677-3596F348F3BE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{DF9FAEE2-ABEC-EA45-9895-DEB78240D50E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="740" windowWidth="27640" windowHeight="16540" xr2:uid="{48BD24B6-4505-BF49-AC82-C339D6D2D38D}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>question_id</t>
   </si>
   <si>
-    <t>resolved</t>
-  </si>
-  <si>
     <t>question_name</t>
   </si>
   <si>
@@ -78,12 +75,6 @@
     <t>Question has fixed 28 day period and the input data were indexed with wrong dates</t>
   </si>
   <si>
-    <t>FALSE, need to add better error; last month of data are dropped</t>
-  </si>
-  <si>
-    <t>FALSE, need to add better error, last month of data are dropped (maybe?)</t>
-  </si>
-  <si>
     <t>How many battle deaths will ACLED record in Afghanistan in April 2018?</t>
   </si>
   <si>
@@ -94,6 +85,15 @@
   </si>
   <si>
     <t>Forecast looks bad, but it's just because the input count series has a lot of 0's and low values, which does not work well for forecaster.</t>
+  </si>
+  <si>
+    <t>resolved_at_PH_end</t>
+  </si>
+  <si>
+    <t>FALSE, last month of data are dropped (maybe?)</t>
+  </si>
+  <si>
+    <t>FALSE, last month of data are dropped</t>
   </si>
 </sst>
 </file>
@@ -449,7 +449,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -463,22 +463,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -492,10 +492,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -512,10 +512,10 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -532,10 +532,10 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -549,10 +549,10 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
         <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -566,10 +566,10 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -583,10 +583,10 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -597,16 +597,16 @@
         <v>938</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -617,16 +617,16 @@
         <v>1055</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
       <c r="F9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixes for 1235, 1406, and 1226
- 1235, 1406: separations errored out because of negative separation values -> fix parse_separations to catch negative values
- 1226: negative forecast values because count series was not recognized, issue was to_lower string did not match "ACLED" keyword, -> fixed keyword to lower as well
</commit_message>
<xml_diff>
--- a/tests/request-issues.xlsx
+++ b/tests/request-issues.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andybega/Work/SAGE-ward-share/basil-ts/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{DF9FAEE2-ABEC-EA45-9895-DEB78240D50E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D1432AA9-3810-8149-9EE2-F2B532FE7637}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="740" windowWidth="27640" windowHeight="16540" xr2:uid="{48BD24B6-4505-BF49-AC82-C339D6D2D38D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>question_id</t>
   </si>
@@ -94,6 +94,48 @@
   </si>
   <si>
     <t>FALSE, last month of data are dropped</t>
+  </si>
+  <si>
+    <t>Will ACLED record any civilian fatalities in Ghana in June 2018?</t>
+  </si>
+  <si>
+    <t>CI was in negative values; series not recognized as count because ACLED keyword was upper case, but ifp name converted to lower when matching</t>
+  </si>
+  <si>
+    <t>problem_at_which_end</t>
+  </si>
+  <si>
+    <t>PH</t>
+  </si>
+  <si>
+    <t>ISI</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>Amandeep</t>
+  </si>
+  <si>
+    <t>What will be the monthly period-over-period change in the consumer price index (CPI) for Benin in April 2018?</t>
+  </si>
+  <si>
+    <t>R error; parse_separations did not recognize negative cutpoints</t>
+  </si>
+  <si>
+    <t>What will be the monthly period-over-period change in the consumer price index (CPI) for Egypt in May 2018?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Will ACLED record any riot/protest events in Gabon in April 2018? </t>
+  </si>
+  <si>
+    <t>R error; parse_separations monotonic check choked on length 1 input for binary IFP</t>
+  </si>
+  <si>
+    <t>5 answer options, but only 4 get back; related to monotonicity check in separations I added</t>
   </si>
 </sst>
 </file>
@@ -446,187 +488,320 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC9EB7E1-8E86-1F4E-9A8E-315E12524CAD}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="64.83203125" customWidth="1"/>
-    <col min="5" max="5" width="63.83203125" customWidth="1"/>
+    <col min="1" max="2" width="11.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="64.83203125" customWidth="1"/>
+    <col min="6" max="6" width="97.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
       <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
       <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43167</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1"/>
+      <c r="C2">
         <v>938</v>
       </c>
-      <c r="C2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43167</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1"/>
+      <c r="C3">
         <v>875</v>
       </c>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43168</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1"/>
+      <c r="C4">
         <v>866</v>
       </c>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43171</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1"/>
+      <c r="C5">
         <v>929</v>
       </c>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43172</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1"/>
+      <c r="C6">
         <v>839</v>
       </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43172</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1"/>
+      <c r="C7">
         <v>821</v>
       </c>
-      <c r="C7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43172</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1"/>
+      <c r="C8">
         <v>938</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>2</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>13</v>
       </c>
-      <c r="F8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43175</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1"/>
+      <c r="C9">
         <v>1055</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>14</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>15</v>
       </c>
-      <c r="F9" t="b">
-        <v>1</v>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>43199</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>1028</v>
+      </c>
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>43201</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <v>839</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>43202</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <v>1235</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>43202</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <v>1406</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>43202</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15">
+        <v>1226</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix plots for cases where aggregation happens in app
</commit_message>
<xml_diff>
--- a/tests/request-issues.xlsx
+++ b/tests/request-issues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andybega/Work/SAGE-ward-share/basil-ts/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D1432AA9-3810-8149-9EE2-F2B532FE7637}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{6AD6B2BE-9F6E-1B45-A848-7F49CE95C823}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="740" windowWidth="27640" windowHeight="16540" xr2:uid="{48BD24B6-4505-BF49-AC82-C339D6D2D38D}"/>
+    <workbookView xWindow="16600" yWindow="7800" windowWidth="27640" windowHeight="16540" xr2:uid="{48BD24B6-4505-BF49-AC82-C339D6D2D38D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>question_id</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>5 answer options, but only 4 get back; related to monotonicity check in separations I added</t>
+  </si>
+  <si>
+    <t>R error; failure to parse date, date had form "in April (Month 04) 2018"</t>
   </si>
 </sst>
 </file>
@@ -491,7 +494,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -709,6 +712,14 @@
         <v>27</v>
       </c>
     </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>1145</v>
+      </c>
+      <c r="F10" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43199</v>

</xml_diff>

<commit_message>
reduce historical data used for training, possible fix for CI issue
</commit_message>
<xml_diff>
--- a/tests/request-issues.xlsx
+++ b/tests/request-issues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andybega/Work/SAGE-ward-share/basil-ts/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andybega/Work/2017-HFC/SAGE-ward-share/basil-ts/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{6AD6B2BE-9F6E-1B45-A848-7F49CE95C823}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D4037BC3-A882-F64D-9845-882FECB5B388}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16600" yWindow="7800" windowWidth="27640" windowHeight="16540" xr2:uid="{48BD24B6-4505-BF49-AC82-C339D6D2D38D}"/>
+    <workbookView xWindow="16580" yWindow="7800" windowWidth="27640" windowHeight="16540" xr2:uid="{48BD24B6-4505-BF49-AC82-C339D6D2D38D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -494,7 +494,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>